<commit_message>
added more for test case 20
</commit_message>
<xml_diff>
--- a/ContactUsData.xlsx
+++ b/ContactUsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yogev/IdeaProjects/Automation_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF6E5E36-C14E-034D-B279-7181F58E7E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB6CFC-3233-CF45-8733-87D468913C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1260" windowWidth="27640" windowHeight="16720" xr2:uid="{29684AA3-8187-B34E-A512-1ED7FFDD01ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>/Users/yogev/IdeaProjects/Automation_Project/theWall.jpg</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>testCase20</t>
+  </si>
+  <si>
+    <t>userName</t>
   </si>
 </sst>
 </file>
@@ -448,15 +457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E985E404-EE28-C048-A194-40145EB59059}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +481,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -488,6 +503,12 @@
       </c>
       <c r="E2" t="s">
         <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>